<commit_message>
Add habitats for figure of PCA and clustering
</commit_message>
<xml_diff>
--- a/output/Clustering/fish/clust_PCs_validity_measures_fish_clean_coda_rob_k4_ward.xlsx
+++ b/output/Clustering/fish/clust_PCs_validity_measures_fish_clean_coda_rob_k4_ward.xlsx
@@ -413,22 +413,22 @@
         <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>0.605</v>
+        <v>0.6</v>
       </c>
       <c r="E2" t="n">
-        <v>0.77</v>
+        <v>0.738</v>
       </c>
       <c r="F2" t="n">
-        <v>0.775</v>
+        <v>0.737</v>
       </c>
       <c r="G2" t="n">
-        <v>0.37</v>
+        <v>0.418</v>
       </c>
       <c r="H2" t="n">
-        <v>1.49</v>
+        <v>1.482</v>
       </c>
       <c r="I2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -442,22 +442,22 @@
         <v>8</v>
       </c>
       <c r="D3" t="n">
-        <v>0.605</v>
+        <v>0.6</v>
       </c>
       <c r="E3" t="n">
-        <v>1.133</v>
+        <v>1.016</v>
       </c>
       <c r="F3" t="n">
-        <v>1.071</v>
+        <v>0.935</v>
       </c>
       <c r="G3" t="n">
-        <v>0.169</v>
+        <v>0.264</v>
       </c>
       <c r="H3" t="n">
-        <v>1.813</v>
+        <v>1.788</v>
       </c>
       <c r="I3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -468,25 +468,25 @@
         <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D4" t="n">
         <v>0.654</v>
       </c>
       <c r="E4" t="n">
-        <v>0.72</v>
+        <v>1.012</v>
       </c>
       <c r="F4" t="n">
-        <v>0.729</v>
+        <v>1.065</v>
       </c>
       <c r="G4" t="n">
-        <v>0.424</v>
+        <v>0.234</v>
       </c>
       <c r="H4" t="n">
-        <v>1.454</v>
+        <v>1.585</v>
       </c>
       <c r="I4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
@@ -497,25 +497,25 @@
         <v>9</v>
       </c>
       <c r="C5" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" t="n">
-        <v>0.668</v>
+        <v>0.628</v>
       </c>
       <c r="E5" t="n">
-        <v>1.223</v>
+        <v>1.123</v>
       </c>
       <c r="F5" t="n">
-        <v>1.3</v>
+        <v>1.067</v>
       </c>
       <c r="G5" t="n">
-        <v>0.15</v>
+        <v>0.257</v>
       </c>
       <c r="H5" t="n">
-        <v>1.906</v>
+        <v>1.909</v>
       </c>
       <c r="I5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>